<commit_message>
New test cases include
</commit_message>
<xml_diff>
--- a/D9-Automation/src/main/java/testData/sampleD9.xlsx
+++ b/D9-Automation/src/main/java/testData/sampleD9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cchitneedi\eclipse-2\D9-Automation\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82388035-CCC8-4DB8-993E-DDC38D036EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C6DF79-9FE3-43E4-9E7D-56FD5900B045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="22" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="30" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="callouts" sheetId="2" r:id="rId1"/>
@@ -38,13 +38,19 @@
     <sheet name="pages" sheetId="23" r:id="rId23"/>
     <sheet name="inputpage" sheetId="24" r:id="rId24"/>
     <sheet name="inputreserve" sheetId="27" r:id="rId25"/>
-    <sheet name="deletereserve" sheetId="28" r:id="rId26"/>
-    <sheet name="research" sheetId="29" r:id="rId27"/>
-    <sheet name="inputresearch" sheetId="30" r:id="rId28"/>
-    <sheet name="deleteresearch" sheetId="31" r:id="rId29"/>
-    <sheet name="indexpage" sheetId="32" r:id="rId30"/>
-    <sheet name="deletepage" sheetId="25" r:id="rId31"/>
-    <sheet name="reserves" sheetId="26" r:id="rId32"/>
+    <sheet name="inputentrytitle" sheetId="36" r:id="rId26"/>
+    <sheet name="deletereserve" sheetId="28" r:id="rId27"/>
+    <sheet name="research" sheetId="29" r:id="rId28"/>
+    <sheet name="inputresearch" sheetId="30" r:id="rId29"/>
+    <sheet name="deleteresearch" sheetId="31" r:id="rId30"/>
+    <sheet name="indexpage" sheetId="32" r:id="rId31"/>
+    <sheet name="inputindextitle" sheetId="33" r:id="rId32"/>
+    <sheet name="deletepage" sheetId="25" r:id="rId33"/>
+    <sheet name="reserves" sheetId="26" r:id="rId34"/>
+    <sheet name="deleteindexpage" sheetId="34" r:id="rId35"/>
+    <sheet name="indexentries" sheetId="35" r:id="rId36"/>
+    <sheet name="deleteindexentry" sheetId="37" r:id="rId37"/>
+    <sheet name="Sheet1" sheetId="38" r:id="rId38"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -56,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="184">
   <si>
     <t>username</t>
   </si>
@@ -64,457 +70,550 @@
     <t>password</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Resource Title</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>SubTitle</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Nilesh</t>
+  </si>
+  <si>
+    <t>Resource Title-31</t>
+  </si>
+  <si>
+    <t>Resource SubTitle-31</t>
+  </si>
+  <si>
+    <t>NESAdmin</t>
+  </si>
+  <si>
+    <t>NESNES</t>
+  </si>
+  <si>
+    <t>Academic Journals Sub-e</t>
+  </si>
+  <si>
+    <t>Academic Journals-e</t>
+  </si>
+  <si>
+    <t>Academic journals from excel</t>
+  </si>
+  <si>
+    <t>Main Title</t>
+  </si>
+  <si>
+    <t>Deletecallout Title</t>
+  </si>
+  <si>
+    <t>pubmed</t>
+  </si>
+  <si>
+    <t>Verizon Research</t>
+  </si>
+  <si>
+    <t>Cred Resarch-M</t>
+  </si>
+  <si>
+    <t>Revision Log</t>
+  </si>
+  <si>
+    <t>Verizon Resource</t>
+  </si>
+  <si>
+    <t>Verizon Resource pvt. Ltd</t>
+  </si>
+  <si>
+    <t>Sharon</t>
+  </si>
+  <si>
+    <t>delete Resource Title</t>
+  </si>
+  <si>
+    <t>ISBN1</t>
+  </si>
+  <si>
+    <t>UPC1</t>
+  </si>
+  <si>
+    <t>SubTitle-1</t>
+  </si>
+  <si>
+    <t>WorkFlow</t>
+  </si>
+  <si>
+    <t>978-3-16-148410-5</t>
+  </si>
+  <si>
+    <t>Cinahal Resources pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>Cinahal process</t>
+  </si>
+  <si>
+    <t>cinahal revison Log</t>
+  </si>
+  <si>
+    <t>Title For Edit</t>
+  </si>
+  <si>
+    <t>Cred Resources</t>
+  </si>
+  <si>
+    <t>Cred Resources pvt ltd</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Cinahal Resources-e</t>
+  </si>
+  <si>
+    <t>EditedTitle</t>
+  </si>
+  <si>
+    <t>External Link</t>
+  </si>
+  <si>
+    <t>DynaMed News Article</t>
+  </si>
+  <si>
+    <t>https://www.google.co.in/</t>
+  </si>
+  <si>
+    <t>Jonny</t>
+  </si>
+  <si>
+    <t>Deleted Callout</t>
+  </si>
+  <si>
+    <t>Work Flow</t>
+  </si>
+  <si>
+    <t>Medline News Article</t>
+  </si>
+  <si>
+    <t>Miraj</t>
+  </si>
+  <si>
+    <t>Umesh</t>
+  </si>
+  <si>
+    <t>Umang News Article work flow</t>
+  </si>
+  <si>
+    <t>Umang - e News Article</t>
+  </si>
+  <si>
+    <t>Title for Edit</t>
+  </si>
+  <si>
+    <t>Edited Title</t>
+  </si>
+  <si>
+    <t>Neliez</t>
+  </si>
+  <si>
+    <t>Delete Custom</t>
+  </si>
+  <si>
+    <t>Cinahal Custom</t>
+  </si>
+  <si>
+    <t>Cinahal Custom revision log</t>
+  </si>
+  <si>
+    <t>Verizon Custom</t>
+  </si>
+  <si>
+    <t>Cred Custom-E</t>
+  </si>
+  <si>
+    <t>Cred Custom-E Log</t>
+  </si>
+  <si>
+    <t>MedLine Listing</t>
+  </si>
+  <si>
+    <t>Main URL</t>
+  </si>
+  <si>
+    <t>SubURL1</t>
+  </si>
+  <si>
+    <t>https://www.stacksdiscovery.com/</t>
+  </si>
+  <si>
+    <t>Pubmed DBL</t>
+  </si>
+  <si>
+    <t>Delete DBL Title</t>
+  </si>
+  <si>
+    <t>Cred DBL-E</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>Sub Title1</t>
+  </si>
+  <si>
+    <t>Sub URL1</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Second Name</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>Project developer</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Edited First Name</t>
+  </si>
+  <si>
+    <t>Edited Second Name</t>
+  </si>
+  <si>
+    <t>Edited Job Title</t>
+  </si>
+  <si>
+    <t>Edited Location</t>
+  </si>
+  <si>
+    <t>Edited Twitter</t>
+  </si>
+  <si>
+    <t>Edited twitterURL</t>
+  </si>
+  <si>
+    <t>DL-E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinahal </t>
+  </si>
+  <si>
+    <t>Production Manager</t>
+  </si>
+  <si>
+    <t>Twitter-E</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Pubmed</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Deleted First Name</t>
+  </si>
+  <si>
+    <t>Page Title</t>
+  </si>
+  <si>
+    <t>Edited Page Title</t>
+  </si>
+  <si>
+    <t>Cinahal-E</t>
+  </si>
+  <si>
+    <t>PubMed Page</t>
+  </si>
+  <si>
+    <t>Deleted Page</t>
+  </si>
+  <si>
+    <t>Reserve Title</t>
+  </si>
+  <si>
+    <t>Registrar Course ID</t>
+  </si>
+  <si>
+    <t>Course ID</t>
+  </si>
+  <si>
+    <t>Medline Reserves</t>
+  </si>
+  <si>
+    <t>MD-RC</t>
+  </si>
+  <si>
+    <t>ID-1</t>
+  </si>
+  <si>
+    <t>Corpus Limited</t>
+  </si>
+  <si>
+    <t>Registrar ID-D</t>
+  </si>
+  <si>
+    <t>Cource ID-D</t>
+  </si>
+  <si>
+    <t>Pubmed Reserve</t>
+  </si>
+  <si>
+    <t>PMD-R</t>
+  </si>
+  <si>
+    <t>PMD-c</t>
+  </si>
+  <si>
+    <t>Delete Reserve</t>
+  </si>
+  <si>
+    <t>Type ddl</t>
+  </si>
+  <si>
+    <t>Tab Name-1</t>
+  </si>
+  <si>
+    <t>DynaMed Plus RG tab-1</t>
+  </si>
+  <si>
+    <t>E-Tab1</t>
+  </si>
+  <si>
+    <t>Research Title</t>
+  </si>
+  <si>
+    <t>PubMed Research</t>
+  </si>
+  <si>
+    <t>Deleted Title</t>
+  </si>
+  <si>
+    <t>Cinahal Index Page</t>
+  </si>
+  <si>
+    <t>SubLinkText1</t>
+  </si>
+  <si>
+    <t>Stacks Discovery</t>
+  </si>
+  <si>
+    <t>Sub-URL1</t>
+  </si>
+  <si>
+    <t>Sub Link1</t>
+  </si>
+  <si>
+    <t>Pubmed Link Text</t>
+  </si>
+  <si>
+    <t>Linkedin URL</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/</t>
+  </si>
+  <si>
+    <t>Linkedin Text</t>
+  </si>
+  <si>
+    <t>Title1 for Edit</t>
+  </si>
+  <si>
+    <t>Title2 for Edit</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>LinkedIn URL</t>
+  </si>
+  <si>
+    <t>Deleted Second Name</t>
+  </si>
+  <si>
+    <t>Revision Log Enterprise Custom</t>
+  </si>
+  <si>
+    <t>DemoType</t>
+  </si>
+  <si>
+    <t>Type DDL</t>
+  </si>
+  <si>
+    <t>Tab URL-1</t>
+  </si>
+  <si>
+    <t>PubMed Research Title</t>
+  </si>
+  <si>
+    <t>E-Tab URL-1</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Corpus Limited Index Page</t>
+  </si>
+  <si>
+    <t>Cinahal Index Page-E</t>
+  </si>
+  <si>
+    <t>Index Page Title</t>
+  </si>
+  <si>
+    <t>Pubmed Index</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Delete Index Title</t>
+  </si>
+  <si>
+    <t>DynaMed Index Entry</t>
+  </si>
+  <si>
+    <t>Index Entry URL</t>
+  </si>
+  <si>
+    <t>Corpus Limited Index Entry</t>
+  </si>
+  <si>
+    <t>Cinahal Index Entry-E</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Index Entry Title</t>
+  </si>
+  <si>
+    <t>PubMed Index Entry</t>
+  </si>
+  <si>
+    <t>IE-URL</t>
+  </si>
+  <si>
+    <t>Index Entry Deleted Title</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>15-04-2022</t>
+  </si>
+  <si>
+    <t>15:21:29</t>
+  </si>
+  <si>
+    <t>16:21:25</t>
+  </si>
+  <si>
+    <t>09:09:09</t>
+  </si>
+  <si>
+    <t>20-05-2022</t>
+  </si>
+  <si>
+    <t>14:15:18</t>
+  </si>
+  <si>
+    <t>Cinahal Page</t>
+  </si>
+  <si>
+    <t>Enterprise Custom</t>
+  </si>
+  <si>
+    <t>DynaMed Plus RG</t>
+  </si>
+  <si>
+    <t>Listing1</t>
+  </si>
+  <si>
+    <t>Excel Callouts-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
     <t>NESadmin</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>subtitle</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Excel Callouts-1</t>
-  </si>
-  <si>
-    <t>Resource Title</t>
-  </si>
-  <si>
-    <t>UPC</t>
-  </si>
-  <si>
-    <t>SubTitle</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Nilesh</t>
-  </si>
-  <si>
     <t>NES2021!</t>
   </si>
   <si>
-    <t>Resource Title-31</t>
-  </si>
-  <si>
-    <t>Resource SubTitle-31</t>
-  </si>
-  <si>
-    <t>NESAdmin</t>
-  </si>
-  <si>
-    <t>NESNES</t>
-  </si>
-  <si>
-    <t>Academic Journals Sub-e</t>
-  </si>
-  <si>
-    <t>Academic Journals-e</t>
-  </si>
-  <si>
-    <t>Academic journals from excel</t>
-  </si>
-  <si>
-    <t>Main Title</t>
-  </si>
-  <si>
-    <t>Deletecallout Title</t>
-  </si>
-  <si>
-    <t>pubmed</t>
-  </si>
-  <si>
-    <t>Verizon Research</t>
-  </si>
-  <si>
-    <t>Cred Resarch-M</t>
-  </si>
-  <si>
-    <t>Revision Log</t>
-  </si>
-  <si>
-    <t>Verizon Resource</t>
-  </si>
-  <si>
-    <t>Verizon Resource pvt. Ltd</t>
-  </si>
-  <si>
-    <t>Sharon</t>
-  </si>
-  <si>
-    <t>delete Resource Title</t>
-  </si>
-  <si>
-    <t>ISBN1</t>
-  </si>
-  <si>
-    <t>UPC1</t>
-  </si>
-  <si>
-    <t>SubTitle-1</t>
-  </si>
-  <si>
-    <t>WorkFlow</t>
-  </si>
-  <si>
-    <t>978-3-16-148410-5</t>
-  </si>
-  <si>
-    <t>Cinahal Resources pvt. Ltd.</t>
-  </si>
-  <si>
-    <t>Cinahal process</t>
-  </si>
-  <si>
-    <t>cinahal revison Log</t>
-  </si>
-  <si>
-    <t>Title For Edit</t>
-  </si>
-  <si>
-    <t>Cred Resources</t>
-  </si>
-  <si>
-    <t>Cred Resources pvt ltd</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Cinahal Resources-e</t>
-  </si>
-  <si>
-    <t>EditedTitle</t>
-  </si>
-  <si>
-    <t>External Link</t>
-  </si>
-  <si>
-    <t>DynaMed News Article</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/</t>
-  </si>
-  <si>
-    <t>Jonny</t>
-  </si>
-  <si>
-    <t>Deleted Callout</t>
-  </si>
-  <si>
-    <t>Work Flow</t>
-  </si>
-  <si>
-    <t>Medline News Article</t>
-  </si>
-  <si>
-    <t>Miraj</t>
-  </si>
-  <si>
-    <t>Umesh</t>
-  </si>
-  <si>
-    <t>Umang News Article work flow</t>
-  </si>
-  <si>
-    <t>Umang - e News Article</t>
-  </si>
-  <si>
-    <t>Title for Edit</t>
-  </si>
-  <si>
-    <t>Edited Title</t>
-  </si>
-  <si>
-    <t>Neliez</t>
-  </si>
-  <si>
-    <t>Enterprise Custom</t>
-  </si>
-  <si>
-    <t>Delete Custom</t>
-  </si>
-  <si>
-    <t>Cinahal Custom</t>
-  </si>
-  <si>
-    <t>Cinahal Custom revision log</t>
-  </si>
-  <si>
-    <t>Verizon Custom</t>
-  </si>
-  <si>
-    <t>Cred Custom-E</t>
-  </si>
-  <si>
-    <t>Cred Custom-E Log</t>
-  </si>
-  <si>
-    <t>MedLine Listing</t>
-  </si>
-  <si>
-    <t>Main URL</t>
-  </si>
-  <si>
-    <t>SubURL1</t>
-  </si>
-  <si>
-    <t>https://www.stacksdiscovery.com/</t>
-  </si>
-  <si>
-    <t>Pubmed DBL</t>
-  </si>
-  <si>
-    <t>Delete DBL Title</t>
-  </si>
-  <si>
-    <t>Cred DBL-E</t>
-  </si>
-  <si>
-    <t>Verizon</t>
-  </si>
-  <si>
-    <t>Sub Title1</t>
-  </si>
-  <si>
-    <t>Sub URL1</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Second Name</t>
-  </si>
-  <si>
-    <t>Job Title</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Directory</t>
-  </si>
-  <si>
-    <t>Listing1</t>
-  </si>
-  <si>
-    <t>Project developer</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Edited First Name</t>
-  </si>
-  <si>
-    <t>Edited Second Name</t>
-  </si>
-  <si>
-    <t>Edited Job Title</t>
-  </si>
-  <si>
-    <t>Edited Location</t>
-  </si>
-  <si>
-    <t>Edited Twitter</t>
-  </si>
-  <si>
-    <t>Edited twitterURL</t>
-  </si>
-  <si>
-    <t>DL-E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cinahal </t>
-  </si>
-  <si>
-    <t>Production Manager</t>
-  </si>
-  <si>
-    <t>Twitter-E</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Pubmed</t>
-  </si>
-  <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>Manager</t>
-  </si>
-  <si>
-    <t>Deleted First Name</t>
-  </si>
-  <si>
-    <t>Page Title</t>
-  </si>
-  <si>
-    <t>Cinahal description Page</t>
-  </si>
-  <si>
-    <t>Edited Page Title</t>
-  </si>
-  <si>
-    <t>Cinahal-E</t>
-  </si>
-  <si>
-    <t>PubMed Page</t>
-  </si>
-  <si>
-    <t>Deleted Page</t>
-  </si>
-  <si>
-    <t>Reserve Title</t>
-  </si>
-  <si>
-    <t>Registrar Course ID</t>
-  </si>
-  <si>
-    <t>Course ID</t>
-  </si>
-  <si>
-    <t>Medline Reserves</t>
-  </si>
-  <si>
-    <t>MD-RC</t>
-  </si>
-  <si>
-    <t>ID-1</t>
-  </si>
-  <si>
-    <t>Corpus Limited</t>
-  </si>
-  <si>
-    <t>E-Registrar ID</t>
-  </si>
-  <si>
-    <t>E-Course ID</t>
-  </si>
-  <si>
-    <t>RGC-ID</t>
-  </si>
-  <si>
-    <t>RCC-ID</t>
-  </si>
-  <si>
-    <t>Registrar ID-D</t>
-  </si>
-  <si>
-    <t>Cource ID-D</t>
-  </si>
-  <si>
-    <t>Pubmed Reserve</t>
-  </si>
-  <si>
-    <t>PMD-R</t>
-  </si>
-  <si>
-    <t>PMD-c</t>
-  </si>
-  <si>
-    <t>Delete Reserve</t>
-  </si>
-  <si>
-    <t>Type ddl</t>
-  </si>
-  <si>
-    <t>Tab Name-1</t>
-  </si>
-  <si>
-    <t>DynaMed Plus RG</t>
-  </si>
-  <si>
-    <t>DynaMed Plus RG tab-1</t>
-  </si>
-  <si>
-    <t>E-Tab1</t>
-  </si>
-  <si>
-    <t>Research Title</t>
-  </si>
-  <si>
-    <t>PubMed Research</t>
-  </si>
-  <si>
-    <t>Deleted Title</t>
-  </si>
-  <si>
-    <t>Cinahal Index Page</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Reviewed</t>
-  </si>
-  <si>
-    <t>IP-WF</t>
-  </si>
-  <si>
-    <t>Cinahal Index Page Work Flow</t>
-  </si>
-  <si>
-    <t>SubLinkText1</t>
-  </si>
-  <si>
-    <t>Stacks Discovery</t>
-  </si>
-  <si>
-    <t>Sub-URL1</t>
-  </si>
-  <si>
-    <t>Sub Link1</t>
-  </si>
-  <si>
-    <t>Pubmed Link Text</t>
-  </si>
-  <si>
-    <t>Linkedin URL</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/</t>
-  </si>
-  <si>
-    <t>Linkedin Text</t>
-  </si>
-  <si>
-    <t>Title1 for Edit</t>
-  </si>
-  <si>
-    <t>Title2 for Edit</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>LinkedIn URL</t>
-  </si>
-  <si>
-    <t>Deleted Second Name</t>
-  </si>
-  <si>
-    <t>Revision Log Enterprise Custom</t>
-  </si>
-  <si>
-    <t>DemoType</t>
-  </si>
-  <si>
-    <t>Type DDL</t>
-  </si>
-  <si>
-    <t>Tab URL-1</t>
-  </si>
-  <si>
-    <t>PubMed Research Title</t>
-  </si>
-  <si>
-    <t>E-Tab URL-1</t>
+    <t>19-06-2022</t>
+  </si>
+  <si>
+    <t>28-04-2022</t>
+  </si>
+  <si>
+    <t>16:21:29</t>
+  </si>
+  <si>
+    <t>17:21:25</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>!@#$7895335</t>
+  </si>
+  <si>
+    <t>9010006190</t>
+  </si>
+  <si>
+    <t>abc@1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -624,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -637,6 +736,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -918,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A696E4-CDE2-4479-91E0-317E4D8124B8}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,12 +1036,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -965,36 +1075,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1">
         <v>360029147</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1008,7 +1118,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,36 +1132,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1077,24 +1187,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1104,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AA02B0-3B6B-4432-B52F-84F38E0E0A00}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,18 +1228,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1157,36 +1275,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1212,24 +1330,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1254,24 +1372,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1282,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D24D4DF-57AB-48F5-B753-BF81C3E59AAA}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,30 +1416,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1348,36 +1480,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>360029145</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1523,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,23 +1542,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>173</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="NES2021@" xr:uid="{6D8F5128-3C21-4588-AA53-E5E53EA41C50}"/>
+    <hyperlink ref="B2" r:id="rId1" display="247@July" xr:uid="{18295E2A-9123-45D0-9F74-9ED027AF83F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1434,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00ACB21D-FE3C-4F55-A325-5FCDD355091A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,18 +1580,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1469,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FE3AD0-0D22-45FB-A3C9-B08544970E9F}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,42 +1627,102 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1551,54 +1751,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1626,54 +1826,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1684,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0BE471-7614-4A95-AF9D-7EA02D36B230}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,12 +1897,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1727,18 +1932,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1749,46 +1954,161 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B951C3-4BAB-4A10-8BFD-C8B0B1F11B21}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C2008D-443D-47EE-853C-AA9AE960E549}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33448B6A-A694-42D0-BC99-E91B612BF17B}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>101</v>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1797,62 +2117,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33448B6A-A694-42D0-BC99-E91B612BF17B}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0355803-D013-4E8F-9CEC-4D5D607D45C6}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,30 +2134,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1896,7 +2180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B00D39-37E1-44F5-BC74-6307284A3A04}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1912,18 +2196,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1932,11 +2216,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AADB152-0E75-4644-9DA7-01A03658FFDB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFAFFD1-95B3-423C-9BCC-F126CABE5CE8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1951,36 +2278,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1989,8 +2316,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AADB152-0E75-4644-9DA7-01A03658FFDB}">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E034048-5913-40E0-98B9-008BF934CAE5}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B877E22-935F-408E-8B02-A9546EF360D1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1999,41 +2369,250 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>50</v>
+        <v>139</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC36548-AD3F-48A0-B209-96AF7E665782}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2D5DFA-FF89-4289-9927-DB81737FA7FC}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E034048-5913-40E0-98B9-008BF934CAE5}">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{D2EE8298-F132-41B6-AB94-9909EDF399F7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34F4420-176D-477A-BFED-52496EDD166E}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2042,66 +2621,134 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>132</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2B2505-9FF6-4CC9-A551-A313FC0AB0A8}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC36548-AD3F-48A0-B209-96AF7E665782}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960FC92A-D28F-49E5-A54B-EA004A3CA663}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>102</v>
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2110,44 +2757,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2D5DFA-FF89-4289-9927-DB81737FA7FC}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4388139F-6724-42D1-8E47-38F4F90E1016}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2167,18 +2784,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2188,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE12593C-B8BB-4423-A368-C6E825C58E5B}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,30 +2821,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>360029145</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="1">
+        <v>360029145</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2253,24 +2884,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2296,30 +2927,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2348,48 +2979,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
         <v>360029146</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2413,18 +3044,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>